<commit_message>
Grade Card Sem 2 v2
Grade Card Sem 2 v2
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 2/Grade Card.xlsx
+++ b/Batch 2018-20/Sem 2/Grade Card.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUOBHAM MURUDKAR\Desktop\SIMSR-Results-Generator-v2-NEW\Batch 2018-20\Sem 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4C5C33-0C35-4231-B894-1F1C013F6491}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DD8D94-71FE-4BDD-A64D-4F4CA92585B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Grade Card" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="PicUp">INDEX([1]Sheet1!$C$2:$C$121,MATCH('Final Grade Card'!$D$13:$I$13,[1]Sheet1!$A$2:$A$121,0))</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>University of Mumbai</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>PATTERN : CHOICE BASED CREDITS &amp; GRADING SYSTEM (CBCSGS)</t>
-  </si>
-  <si>
-    <t>#10</t>
   </si>
   <si>
     <t>PROGRAMME : MASTER OF MANAGEMENT STUDIES (SEMESTER - II)</t>
@@ -303,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -313,11 +310,74 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -340,68 +400,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -500,7 +500,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2140"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2142"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -26942,6 +26942,24 @@
           <cell r="BD123" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE123">
+            <v>4</v>
+          </cell>
+          <cell r="BF123">
+            <v>0</v>
+          </cell>
+          <cell r="BG123">
+            <v>0</v>
+          </cell>
+          <cell r="BH123">
+            <v>0</v>
+          </cell>
+          <cell r="BI123">
+            <v>0</v>
+          </cell>
+          <cell r="BJ123">
+            <v>0</v>
+          </cell>
         </row>
         <row r="124">
           <cell r="A124" t="str">
@@ -27112,6 +27130,24 @@
           <cell r="BD124" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE124">
+            <v>4</v>
+          </cell>
+          <cell r="BF124">
+            <v>0</v>
+          </cell>
+          <cell r="BG124">
+            <v>0</v>
+          </cell>
+          <cell r="BH124">
+            <v>0</v>
+          </cell>
+          <cell r="BI124">
+            <v>0</v>
+          </cell>
+          <cell r="BJ124">
+            <v>0</v>
+          </cell>
         </row>
         <row r="125">
           <cell r="A125" t="str">
@@ -27282,6 +27318,24 @@
           <cell r="BD125" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE125">
+            <v>4</v>
+          </cell>
+          <cell r="BF125">
+            <v>0</v>
+          </cell>
+          <cell r="BG125">
+            <v>0</v>
+          </cell>
+          <cell r="BH125">
+            <v>0</v>
+          </cell>
+          <cell r="BI125">
+            <v>0</v>
+          </cell>
+          <cell r="BJ125">
+            <v>0</v>
+          </cell>
         </row>
         <row r="126">
           <cell r="A126" t="str">
@@ -27452,6 +27506,24 @@
           <cell r="BD126" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE126">
+            <v>4</v>
+          </cell>
+          <cell r="BF126">
+            <v>0</v>
+          </cell>
+          <cell r="BG126">
+            <v>0</v>
+          </cell>
+          <cell r="BH126">
+            <v>0</v>
+          </cell>
+          <cell r="BI126">
+            <v>0</v>
+          </cell>
+          <cell r="BJ126">
+            <v>0</v>
+          </cell>
         </row>
         <row r="127">
           <cell r="A127" t="str">
@@ -27622,6 +27694,24 @@
           <cell r="BD127" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE127">
+            <v>4</v>
+          </cell>
+          <cell r="BF127">
+            <v>0</v>
+          </cell>
+          <cell r="BG127">
+            <v>0</v>
+          </cell>
+          <cell r="BH127">
+            <v>0</v>
+          </cell>
+          <cell r="BI127">
+            <v>0</v>
+          </cell>
+          <cell r="BJ127">
+            <v>0</v>
+          </cell>
         </row>
         <row r="128">
           <cell r="A128" t="str">
@@ -27792,6 +27882,24 @@
           <cell r="BD128" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE128">
+            <v>4</v>
+          </cell>
+          <cell r="BF128">
+            <v>0</v>
+          </cell>
+          <cell r="BG128">
+            <v>0</v>
+          </cell>
+          <cell r="BH128">
+            <v>0</v>
+          </cell>
+          <cell r="BI128">
+            <v>0</v>
+          </cell>
+          <cell r="BJ128">
+            <v>0</v>
+          </cell>
         </row>
         <row r="129">
           <cell r="A129" t="str">
@@ -27962,6 +28070,24 @@
           <cell r="BD129" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE129">
+            <v>4</v>
+          </cell>
+          <cell r="BF129">
+            <v>0</v>
+          </cell>
+          <cell r="BG129">
+            <v>0</v>
+          </cell>
+          <cell r="BH129">
+            <v>0</v>
+          </cell>
+          <cell r="BI129">
+            <v>0</v>
+          </cell>
+          <cell r="BJ129">
+            <v>0</v>
+          </cell>
         </row>
         <row r="130">
           <cell r="A130" t="str">
@@ -28132,6 +28258,24 @@
           <cell r="BD130" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE130">
+            <v>4</v>
+          </cell>
+          <cell r="BF130">
+            <v>0</v>
+          </cell>
+          <cell r="BG130">
+            <v>0</v>
+          </cell>
+          <cell r="BH130">
+            <v>0</v>
+          </cell>
+          <cell r="BI130">
+            <v>0</v>
+          </cell>
+          <cell r="BJ130">
+            <v>0</v>
+          </cell>
         </row>
         <row r="131">
           <cell r="A131" t="str">
@@ -28302,6 +28446,24 @@
           <cell r="BD131" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE131">
+            <v>4</v>
+          </cell>
+          <cell r="BF131">
+            <v>0</v>
+          </cell>
+          <cell r="BG131">
+            <v>0</v>
+          </cell>
+          <cell r="BH131">
+            <v>0</v>
+          </cell>
+          <cell r="BI131">
+            <v>0</v>
+          </cell>
+          <cell r="BJ131">
+            <v>0</v>
+          </cell>
         </row>
         <row r="132">
           <cell r="A132" t="str">
@@ -28472,6 +28634,24 @@
           <cell r="BD132" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE132">
+            <v>4</v>
+          </cell>
+          <cell r="BF132">
+            <v>0</v>
+          </cell>
+          <cell r="BG132">
+            <v>0</v>
+          </cell>
+          <cell r="BH132">
+            <v>0</v>
+          </cell>
+          <cell r="BI132">
+            <v>0</v>
+          </cell>
+          <cell r="BJ132">
+            <v>0</v>
+          </cell>
         </row>
         <row r="133">
           <cell r="A133" t="str">
@@ -28642,6 +28822,24 @@
           <cell r="BD133" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE133">
+            <v>4</v>
+          </cell>
+          <cell r="BF133">
+            <v>0</v>
+          </cell>
+          <cell r="BG133">
+            <v>0</v>
+          </cell>
+          <cell r="BH133">
+            <v>0</v>
+          </cell>
+          <cell r="BI133">
+            <v>0</v>
+          </cell>
+          <cell r="BJ133">
+            <v>0</v>
+          </cell>
         </row>
         <row r="134">
           <cell r="A134" t="str">
@@ -28812,6 +29010,24 @@
           <cell r="BD134" t="str">
             <v>0</v>
           </cell>
+          <cell r="BE134">
+            <v>4</v>
+          </cell>
+          <cell r="BF134">
+            <v>0</v>
+          </cell>
+          <cell r="BG134">
+            <v>0</v>
+          </cell>
+          <cell r="BH134">
+            <v>0</v>
+          </cell>
+          <cell r="BI134">
+            <v>0</v>
+          </cell>
+          <cell r="BJ134">
+            <v>0</v>
+          </cell>
         </row>
         <row r="135">
           <cell r="A135" t="str">
@@ -28980,6 +29196,24 @@
             <v>F</v>
           </cell>
           <cell r="BD135" t="str">
+            <v>0</v>
+          </cell>
+          <cell r="BE135">
+            <v>4</v>
+          </cell>
+          <cell r="BF135">
+            <v>0</v>
+          </cell>
+          <cell r="BG135">
+            <v>0</v>
+          </cell>
+          <cell r="BH135">
+            <v>0</v>
+          </cell>
+          <cell r="BI135">
+            <v>0</v>
+          </cell>
+          <cell r="BJ135">
             <v>0</v>
           </cell>
         </row>
@@ -53321,59 +53555,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
@@ -53387,154 +53621,154 @@
       <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="str">
+      <c r="A9" s="14" t="str">
         <f>"NAME OF THE CANDIDATE : "&amp;VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
         <v>NAME OF THE CANDIDATE : ADEPU CHETAN GANESH ARCHANA</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>19</v>
+      <c r="A10" s="14" t="s">
+        <v>18</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="23" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="20" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="19" t="str">
+      <c r="B17" s="21" t="str">
         <f>'[2]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
       <c r="E17" s="4">
         <v>4</v>
       </c>
@@ -53558,12 +53792,12 @@
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="19" t="str">
+      <c r="B18" s="21" t="str">
         <f>'[2]Subjects List'!$C$5</f>
         <v>Financial Accounting</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="4">
         <v>4</v>
       </c>
@@ -53587,12 +53821,12 @@
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="19" t="str">
+      <c r="B19" s="21" t="str">
         <f>'[2]Subjects List'!$C$6</f>
         <v>Business Statistics</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="4">
         <v>4</v>
       </c>
@@ -53616,12 +53850,12 @@
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="19" t="str">
+      <c r="B20" s="21" t="str">
         <f>'[2]Subjects List'!$C$7</f>
         <v>Operations Management</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="4">
         <v>4</v>
       </c>
@@ -53645,12 +53879,12 @@
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="19" t="str">
+      <c r="B21" s="21" t="str">
         <f>'[2]Subjects List'!$C$8</f>
         <v>Managerial Economics</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="4">
         <v>4</v>
       </c>
@@ -53674,12 +53908,12 @@
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="19" t="str">
+      <c r="B22" s="21" t="str">
         <f>'[2]Subjects List'!$C$9</f>
         <v>Effective and Management Communication</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="4">
         <v>4</v>
       </c>
@@ -53703,12 +53937,12 @@
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="19" t="str">
+      <c r="B23" s="21" t="str">
         <f>'[2]Subjects List'!$C$10</f>
         <v>Negotiation and Selling Skills</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="4">
         <v>4</v>
       </c>
@@ -53732,12 +53966,12 @@
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="19" t="str">
+      <c r="B24" s="21" t="str">
         <f>'[2]Subjects List'!$C$11</f>
         <v>Organisational Behaviour</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="4">
         <v>4</v>
       </c>
@@ -53757,64 +53991,68 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="5">
+      <c r="C25" s="13"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="35">
         <f>SUM(G17:G24)</f>
         <v>32</v>
       </c>
-      <c r="H25" s="30" t="s">
-        <v>18</v>
+      <c r="H25" s="7">
+        <f>VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BJ$135,62,0)</f>
+        <v>66</v>
       </c>
-      <c r="I25" s="3"/>
+      <c r="I25" s="7">
+        <f>SUM(I17:I24)</f>
+        <v>264</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="str">
+      <c r="A26" s="28" t="str">
         <f>"Remark    :  "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BM$122,65,0)</f>
         <v>Remark    :  Unsuccessful</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="27" t="str">
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="22" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI : 8.25</v>
       </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="10" t="str">
+      <c r="F26" s="23"/>
+      <c r="G26" s="31" t="str">
         <f>"Overall Grade : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BO$122,67,0)</f>
         <v>Overall Grade : A</v>
       </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="6" t="str">
+      <c r="H26" s="32"/>
+      <c r="I26" s="5" t="str">
         <f>"Range : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BP$122,68,0)</f>
         <v>Range : 70-74.99</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="28" t="str">
+      <c r="D27" s="12"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="13" t="str">
         <f>"SGPI (I) : "&amp;VLOOKUP(D13,'[4]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI (I) : 8.25</v>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="32"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28"/>
@@ -53889,38 +54127,58 @@
       <c r="I33"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="33" t="s">
-        <v>20</v>
+      <c r="A34" s="11" t="s">
+        <v>19</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="70dE8NwkGWuyHizmxT3wI8Eed8eLNFh1f3cC/W6TJqv/pAIm/qgapMxV9X2N4QzKEBR4kD2FpaWiArNW9SjzwA==" saltValue="L7VzVvx7saQmRFj8j/8L+Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="inYUFqhrCAag0id0HlYSttzgS9wPV9SKb/FbC3yh2bX6ik1kxOInqmEz9zG7iex5K5Y6qApmfWCeatRhANgNcQ==" saltValue="8RJvGAvSja/ZdR2QmpB3MQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="H25" name="Hash Tag 10"/>
+    <protectedRange sqref="C27" name="Declared Date"/>
+    <protectedRange sqref="D13" name="Seat No."/>
     <protectedRange sqref="A11" name="Held In"/>
-    <protectedRange sqref="D13" name="Seat No."/>
-    <protectedRange sqref="C27" name="Declared Date"/>
+    <protectedRange sqref="F25" name="Hash Tag 10"/>
   </protectedRanges>
   <mergeCells count="36">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:I5"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A26:D26"/>
     <mergeCell ref="A34:I35"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="G27:H27"/>
@@ -53937,26 +54195,6 @@
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A1:I5"/>
   </mergeCells>
   <pageMargins left="0.69" right="0" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Delete Backup and Update GC
Delete Old Backup and Update Grade Card to New
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 2/Grade Card.xlsx
+++ b/Batch 2018-20/Sem 2/Grade Card.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUOBHAM MURUDKAR\Desktop\SIMSR-Results-Generator-v2-NEW\Batch 2018-20\Sem 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhishek Chitnis\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DD8D94-71FE-4BDD-A64D-4F4CA92585B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C3E2862-64F2-4EFF-9CF3-987B98161B42}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Grade Card" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="PicUp">INDEX([1]Sheet1!$C$2:$C$121,MATCH('Final Grade Card'!$D$13:$I$13,[1]Sheet1!$A$2:$A$121,0))</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -328,38 +328,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,14 +337,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -388,19 +388,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -500,7 +500,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2142"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2143"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -53555,220 +53555,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="34"/>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="str">
+      <c r="A9" s="32" t="str">
         <f>"NAME OF THE CANDIDATE : "&amp;VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
         <v>NAME OF THE CANDIDATE : ADEPU CHETAN GANESH ARCHANA</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="14" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="21" t="str">
+      <c r="B17" s="24" t="str">
         <f>'[2]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="4">
         <v>4</v>
       </c>
@@ -53792,12 +53792,12 @@
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="21" t="str">
+      <c r="B18" s="24" t="str">
         <f>'[2]Subjects List'!$C$5</f>
         <v>Financial Accounting</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="4">
         <v>4</v>
       </c>
@@ -53821,12 +53821,12 @@
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="21" t="str">
+      <c r="B19" s="24" t="str">
         <f>'[2]Subjects List'!$C$6</f>
         <v>Business Statistics</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="4">
         <v>4</v>
       </c>
@@ -53850,12 +53850,12 @@
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="21" t="str">
+      <c r="B20" s="24" t="str">
         <f>'[2]Subjects List'!$C$7</f>
         <v>Operations Management</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
       <c r="E20" s="4">
         <v>4</v>
       </c>
@@ -53879,12 +53879,12 @@
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="21" t="str">
+      <c r="B21" s="24" t="str">
         <f>'[2]Subjects List'!$C$8</f>
         <v>Managerial Economics</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="4">
         <v>4</v>
       </c>
@@ -53908,12 +53908,12 @@
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="21" t="str">
+      <c r="B22" s="24" t="str">
         <f>'[2]Subjects List'!$C$9</f>
         <v>Effective and Management Communication</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
       <c r="E22" s="4">
         <v>4</v>
       </c>
@@ -53937,12 +53937,12 @@
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="21" t="str">
+      <c r="B23" s="24" t="str">
         <f>'[2]Subjects List'!$C$10</f>
         <v>Negotiation and Selling Skills</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="4">
         <v>4</v>
       </c>
@@ -53966,12 +53966,12 @@
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="21" t="str">
+      <c r="B24" s="24" t="str">
         <f>'[2]Subjects List'!$C$11</f>
         <v>Organisational Behaviour</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="4">
         <v>4</v>
       </c>
@@ -53993,14 +53993,14 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="23"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="8"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="35">
+      <c r="G25" s="11">
         <f>SUM(G17:G24)</f>
         <v>32</v>
       </c>
@@ -54021,37 +54021,37 @@
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
       <c r="D26" s="30"/>
-      <c r="E26" s="22" t="str">
+      <c r="E26" s="12" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI : 8.25</v>
       </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="31" t="str">
+      <c r="F26" s="13"/>
+      <c r="G26" s="14" t="str">
         <f>"Overall Grade : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BO$122,67,0)</f>
         <v>Overall Grade : A</v>
       </c>
-      <c r="H26" s="32"/>
+      <c r="H26" s="15"/>
       <c r="I26" s="5" t="str">
         <f>"Range : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BP$122,68,0)</f>
         <v>Range : 70-74.99</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="12"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="13" t="str">
+      <c r="G27" s="18" t="str">
         <f>"SGPI (I) : "&amp;VLOOKUP(D13,'[4]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI (I) : 8.25</v>
       </c>
-      <c r="H27" s="13"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -54097,10 +54097,10 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I31" s="17"/>
+      <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -54127,28 +54127,28 @@
       <c r="I33"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="inYUFqhrCAag0id0HlYSttzgS9wPV9SKb/FbC3yh2bX6ik1kxOInqmEz9zG7iex5K5Y6qApmfWCeatRhANgNcQ==" saltValue="8RJvGAvSja/ZdR2QmpB3MQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
@@ -54159,26 +54159,6 @@
     <protectedRange sqref="F25" name="Hash Tag 10"/>
   </protectedRanges>
   <mergeCells count="36">
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A1:I5"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A26:D26"/>
     <mergeCell ref="A34:I35"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="G27:H27"/>
@@ -54195,6 +54175,26 @@
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:I5"/>
+    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <pageMargins left="0.69" right="0" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>